<commit_message>
Issues fixed and updated the excel.
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker.xlsx
+++ b/docs/QA/Issue tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Technogy" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="355">
   <si>
     <t>Issue</t>
   </si>
@@ -2123,6 +2123,15 @@
   </si>
   <si>
     <t>ARK28</t>
+  </si>
+  <si>
+    <t>Fixed. Need to be retested by QA.</t>
+  </si>
+  <si>
+    <t>It has become responsive. Need not fix issues.</t>
+  </si>
+  <si>
+    <t>UI alignment.Looking  Same as en/us page. Nothing to fix.</t>
   </si>
 </sst>
 </file>
@@ -2354,14 +2363,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2384,6 +2401,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2393,17 +2413,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3439,10 +3448,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="35" t="s">
         <v>282</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -3465,8 +3474,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="30"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="17" t="s">
         <v>280</v>
       </c>
@@ -3503,7 +3512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -3920,13 +3929,13 @@
       <c r="B16" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="30" t="s">
         <v>300</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -3952,7 +3961,7 @@
       <c r="D17" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="30" t="s">
         <v>300</v>
       </c>
       <c r="F17" s="10" t="s">
@@ -3978,7 +3987,7 @@
       <c r="D18" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="30" t="s">
         <v>300</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -4004,7 +4013,7 @@
       <c r="D19" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="30" t="s">
         <v>300</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -4030,7 +4039,7 @@
       <c r="D20" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="30" t="s">
         <v>300</v>
       </c>
       <c r="F20" s="10" t="s">
@@ -4056,7 +4065,7 @@
       <c r="D21" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="30" t="s">
         <v>300</v>
       </c>
       <c r="F21" s="10" t="s">
@@ -4200,80 +4209,80 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="33" t="s">
         <v>338</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="33" t="s">
         <v>341</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="32" t="s">
         <v>342</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="32" t="s">
         <v>343</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="34">
         <v>42360</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="46" t="s">
+      <c r="G27" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="H27" s="46" t="s">
+      <c r="H27" s="33" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="32" t="s">
         <v>346</v>
       </c>
-      <c r="E28" s="47">
+      <c r="E28" s="34">
         <v>42360</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="46" t="s">
+      <c r="G28" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="H28" s="46" t="s">
+      <c r="H28" s="33" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="33" t="s">
         <v>351</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="33" t="s">
         <v>347</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="32" t="s">
         <v>348</v>
       </c>
-      <c r="D29" s="45" t="s">
+      <c r="D29" s="32" t="s">
         <v>349</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="34">
         <v>42360</v>
       </c>
-      <c r="F29" s="46" t="s">
+      <c r="F29" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="H29" s="46" t="s">
+      <c r="H29" s="33" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4495,10 +4504,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -4518,8 +4527,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="8" t="s">
         <v>100</v>
       </c>
@@ -4537,8 +4546,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="10" t="s">
         <v>100</v>
       </c>
@@ -4556,10 +4565,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="41" t="s">
         <v>110</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -4579,8 +4588,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="8" t="s">
         <v>102</v>
       </c>
@@ -4598,8 +4607,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="10" t="s">
         <v>104</v>
       </c>
@@ -4617,8 +4626,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="8" t="s">
         <v>106</v>
       </c>
@@ -4636,8 +4645,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="8" t="s">
         <v>108</v>
       </c>
@@ -4704,10 +4713,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="44" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -4727,8 +4736,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="8" t="s">
         <v>102</v>
       </c>
@@ -4746,8 +4755,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="8" t="s">
         <v>108</v>
       </c>
@@ -4765,8 +4774,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="32"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="10" t="s">
         <v>106</v>
       </c>
@@ -4807,10 +4816,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="44" t="s">
         <v>116</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -4830,8 +4839,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="32"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="10" t="s">
         <v>104</v>
       </c>
@@ -4964,10 +4973,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="44" t="s">
         <v>126</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -4987,8 +4996,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="44"/>
       <c r="C25" s="10" t="s">
         <v>120</v>
       </c>
@@ -5099,16 +5108,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -5205,10 +5214,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="46" t="s">
         <v>226</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -5228,8 +5237,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="17" t="s">
         <v>227</v>
       </c>
@@ -5247,8 +5256,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="17" t="s">
         <v>229</v>
       </c>
@@ -5266,7 +5275,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="36" t="s">
         <v>231</v>
       </c>
       <c r="B6" s="17" t="s">
@@ -5289,7 +5298,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="36"/>
       <c r="C7" s="17" t="s">
         <v>227</v>
       </c>
@@ -5353,10 +5362,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>240</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -5376,8 +5385,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="17" t="s">
         <v>229</v>
       </c>
@@ -5479,8 +5488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5520,7 +5529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>190</v>
       </c>
@@ -5543,9 +5552,11 @@
         <v>99</v>
       </c>
       <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I2" s="33" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>191</v>
       </c>
@@ -5568,7 +5579,9 @@
         <v>99</v>
       </c>
       <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="I3" s="33" t="s">
+        <v>352</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5579,8 +5592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5590,7 +5603,9 @@
     <col min="3" max="3" width="53.5703125" style="17" customWidth="1"/>
     <col min="4" max="4" width="53.7109375" style="17" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="17" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="17"/>
+    <col min="6" max="8" width="9.140625" style="17"/>
+    <col min="9" max="9" width="43.85546875" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5623,10 +5638,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="46" t="s">
         <v>226</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -5644,10 +5659,13 @@
       <c r="G2" s="17" t="s">
         <v>99</v>
       </c>
+      <c r="I2" s="33" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="17" t="s">
         <v>260</v>
       </c>
@@ -5663,10 +5681,13 @@
       <c r="G3" s="17" t="s">
         <v>99</v>
       </c>
+      <c r="I3" s="33" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="17" t="s">
         <v>262</v>
       </c>
@@ -5681,6 +5702,9 @@
       </c>
       <c r="G4" s="17" t="s">
         <v>99</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5705,6 +5729,7 @@
       <c r="G5" s="17" t="s">
         <v>99</v>
       </c>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -5727,6 +5752,9 @@
       </c>
       <c r="G6" s="17" t="s">
         <v>99</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed issues in architecture variations and updated with developer comments
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker.xlsx
+++ b/docs/QA/Issue tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="468" windowWidth="14808" windowHeight="7656" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Technogy" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Benifits" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Architecture!$A$1:$I$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Architecture!$A$1:$I$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Product landing new'!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Technogy!$A$1:$I$8</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="367">
   <si>
     <t>Issue</t>
   </si>
@@ -2132,6 +2132,45 @@
   </si>
   <si>
     <t>UI alignment.Looking  Same as en/us page. Nothing to fix.</t>
+  </si>
+  <si>
+    <t>List and tile boredered components are not having image property to set these images</t>
+  </si>
+  <si>
+    <t>1) (PDF , 467 KB) - we are not setting this html as is. We are extracting PDF and 467 KB seperately and in Chard we are having separate properties to set these values seperately. So as per AEM logic it is displaying as (PDF - 467 KB). We can see the same in en/us page also.
+2) List and tile boredered components are not having image property to set these images</t>
+  </si>
+  <si>
+    <t>Checked with Priyanka.This is not an issue.</t>
+  </si>
+  <si>
+    <t>This issue is reported in report. Please check</t>
+  </si>
+  <si>
+    <t>Fixed and need to checkin the code</t>
+  </si>
+  <si>
+    <t>put it in general observations list</t>
+  </si>
+  <si>
+    <t>1. Issue is reported in the report.Please check
+2.put it in general observations list
+3.UI is similar to en/us page. So this is not an issue</t>
+  </si>
+  <si>
+    <t>This should be in observations list</t>
+  </si>
+  <si>
+    <t>Checked with Ajay.This is not an issue.</t>
+  </si>
+  <si>
+    <t>UI is similar to en/us page. So this is not an issue</t>
+  </si>
+  <si>
+    <t>Issue is reported in the report.Please check. As Text Element is not found on web publisher page, whatever there in CQ text node is coming on page</t>
+  </si>
+  <si>
+    <t>Not an issue</t>
   </si>
 </sst>
 </file>
@@ -2380,6 +2419,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2400,9 +2442,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2722,17 +2761,17 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
     <col min="2" max="2" width="51" style="3" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="51.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.109375" style="3"/>
+    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2983,21 +3022,21 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="3"/>
+    <col min="7" max="7" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="10" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3104,7 +3143,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -3156,7 +3195,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
@@ -3208,7 +3247,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>75</v>
       </c>
@@ -3260,7 +3299,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>77</v>
       </c>
@@ -3309,7 +3348,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>292</v>
       </c>
@@ -3332,7 +3371,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>293</v>
       </c>
@@ -3355,7 +3394,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>294</v>
       </c>
@@ -3378,7 +3417,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>295</v>
       </c>
@@ -3401,7 +3440,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="27" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="27" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>296</v>
       </c>
@@ -3424,7 +3463,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>297</v>
       </c>
@@ -3447,7 +3486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
         <v>298</v>
       </c>
@@ -3473,7 +3512,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
       <c r="B20" s="35"/>
       <c r="C20" s="17" t="s">
@@ -3512,24 +3551,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="11.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="51.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.109375" style="3"/>
+    <col min="8" max="8" width="11.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3555,7 +3594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>43</v>
       </c>
@@ -3610,7 +3649,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>87</v>
       </c>
@@ -3635,8 +3674,11 @@
       <c r="H4" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I4" s="33" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>88</v>
       </c>
@@ -3662,7 +3704,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>147</v>
       </c>
@@ -3688,7 +3730,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>148</v>
       </c>
@@ -3714,7 +3756,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>149</v>
       </c>
@@ -3740,7 +3782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>168</v>
       </c>
@@ -3765,8 +3807,11 @@
       <c r="H9" s="17" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I9" s="33" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>173</v>
       </c>
@@ -3791,8 +3836,11 @@
       <c r="H10" s="17" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="33" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>178</v>
       </c>
@@ -3818,7 +3866,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>180</v>
       </c>
@@ -3843,8 +3891,11 @@
       <c r="H12" s="17" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I12" s="33" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>182</v>
       </c>
@@ -3869,8 +3920,11 @@
       <c r="H13" s="17" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>217</v>
       </c>
@@ -3895,8 +3949,11 @@
       <c r="H14" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="I14" s="33" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>218</v>
       </c>
@@ -3921,8 +3978,11 @@
       <c r="H15" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+      <c r="I15" s="33" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>327</v>
       </c>
@@ -3947,8 +4007,11 @@
       <c r="H16" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="I16" s="33" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>328</v>
       </c>
@@ -3973,8 +4036,11 @@
       <c r="H17" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I17" s="33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>329</v>
       </c>
@@ -3999,8 +4065,11 @@
       <c r="H18" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I18" s="33" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>330</v>
       </c>
@@ -4025,8 +4094,11 @@
       <c r="H19" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="I19" s="33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>331</v>
       </c>
@@ -4051,8 +4123,11 @@
       <c r="H20" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I20" s="33" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>332</v>
       </c>
@@ -4077,8 +4152,11 @@
       <c r="H21" s="3" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I21" s="33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>333</v>
       </c>
@@ -4103,8 +4181,11 @@
       <c r="H22" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I22" s="33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>334</v>
       </c>
@@ -4129,8 +4210,11 @@
       <c r="H23" s="3" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I23" s="33" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
         <v>335</v>
       </c>
@@ -4155,8 +4239,11 @@
       <c r="H24" s="3" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I24" s="33" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>336</v>
       </c>
@@ -4181,8 +4268,11 @@
       <c r="H25" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I25" s="33" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
         <v>337</v>
       </c>
@@ -4207,8 +4297,11 @@
       <c r="H26" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I26" s="33" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
         <v>338</v>
       </c>
@@ -4233,8 +4326,11 @@
       <c r="H27" s="33" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I27" s="33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
         <v>350</v>
       </c>
@@ -4259,8 +4355,11 @@
       <c r="H28" s="33" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="33" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>351</v>
       </c>
@@ -4285,8 +4384,12 @@
       <c r="H29" s="33" t="s">
         <v>47</v>
       </c>
+      <c r="I29" s="33" t="s">
+        <v>366</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I29"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>
@@ -4309,13 +4412,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4344,7 +4447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>163</v>
       </c>
@@ -4367,7 +4470,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>164</v>
       </c>
@@ -4409,7 +4512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>166</v>
       </c>
@@ -4432,7 +4535,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>167</v>
       </c>
@@ -4468,16 +4571,16 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="3"/>
-    <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="68.28515625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="16.28515625" style="3"/>
+    <col min="1" max="1" width="16.33203125" style="3"/>
+    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="68.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="16.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4503,11 +4606,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -4526,9 +4629,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="39"/>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="38"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="8" t="s">
         <v>100</v>
       </c>
@@ -4545,9 +4648,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="40"/>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="38"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="10" t="s">
         <v>100</v>
       </c>
@@ -4564,11 +4667,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>110</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -4587,9 +4690,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="41"/>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="44"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="8" t="s">
         <v>102</v>
       </c>
@@ -4606,9 +4709,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="41"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="44"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="10" t="s">
         <v>104</v>
       </c>
@@ -4625,9 +4728,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="41"/>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="44"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="8" t="s">
         <v>106</v>
       </c>
@@ -4644,9 +4747,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="41"/>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="44"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="8" t="s">
         <v>108</v>
       </c>
@@ -4712,11 +4815,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="37" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -4735,9 +4838,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="44"/>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="38"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="8" t="s">
         <v>102</v>
       </c>
@@ -4754,9 +4857,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="44"/>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="8" t="s">
         <v>108</v>
       </c>
@@ -4773,9 +4876,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="44"/>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="38"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="10" t="s">
         <v>106</v>
       </c>
@@ -4815,11 +4918,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="37" t="s">
         <v>116</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -4838,9 +4941,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="44"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="38"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="10" t="s">
         <v>104</v>
       </c>
@@ -4972,11 +5075,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="37" t="s">
         <v>126</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -4995,9 +5098,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="44"/>
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="38"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="10" t="s">
         <v>120</v>
       </c>
@@ -5108,16 +5211,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B12:B15"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -5151,14 +5254,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.85546875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="8.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.88671875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5213,7 +5316,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>225</v>
       </c>
@@ -5236,7 +5339,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="45"/>
       <c r="B4" s="46"/>
       <c r="C4" s="17" t="s">
@@ -5255,7 +5358,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" s="46"/>
       <c r="C5" s="17" t="s">
@@ -5274,7 +5377,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>231</v>
       </c>
@@ -5297,7 +5400,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
       <c r="C7" s="17" t="s">
         <v>227</v>
@@ -5361,7 +5464,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
         <v>239</v>
       </c>
@@ -5384,7 +5487,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="46"/>
       <c r="B11" s="47"/>
       <c r="C11" s="17" t="s">
@@ -5449,7 +5552,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>247</v>
       </c>
@@ -5492,12 +5595,12 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="67.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5592,20 +5695,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="52.140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="17" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="17"/>
-    <col min="9" max="9" width="43.85546875" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.109375" style="17"/>
+    <col min="2" max="2" width="52.109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="17" customWidth="1"/>
+    <col min="6" max="8" width="9.109375" style="17"/>
+    <col min="9" max="9" width="43.88671875" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5637,7 +5740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>163</v>
       </c>
@@ -5663,7 +5766,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="45"/>
       <c r="B3" s="46"/>
       <c r="C3" s="17" t="s">
@@ -5685,7 +5788,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="45"/>
       <c r="B4" s="46"/>
       <c r="C4" s="17" t="s">
@@ -5843,11 +5946,11 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.5546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated comment to fix the issue with the image migration.
</commit_message>
<xml_diff>
--- a/docs/QA/Issue tracker.xlsx
+++ b/docs/QA/Issue tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="525" windowWidth="14805" windowHeight="7590" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="525" windowWidth="14805" windowHeight="7590" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Technogy" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="378">
   <si>
     <t>Issue</t>
   </si>
@@ -2723,6 +2723,9 @@
   </si>
   <si>
     <t>Has to be retested. Not reproducible as of now.</t>
+  </si>
+  <si>
+    <t>issue with the content node structure, this should be fixed with updated content.</t>
   </si>
 </sst>
 </file>
@@ -2970,21 +2973,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3046,6 +3034,21 @@
       <alignment horizontal="justify"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3056,6 +3059,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3104,7 +3110,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3139,7 +3145,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3923,7 +3929,7 @@
       <c r="A12" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="31" t="s">
         <v>354</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -4081,10 +4087,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="57" t="s">
         <v>278</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="56" t="s">
         <v>359</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -4107,8 +4113,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="17" t="s">
         <v>265</v>
       </c>
@@ -5161,20 +5167,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+    <sheetView topLeftCell="B19" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="40" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="59" customWidth="1"/>
-    <col min="3" max="9" width="10.7109375" style="40" customWidth="1"/>
-    <col min="10" max="16384" width="10.7109375" style="40"/>
+    <col min="1" max="1" width="10.7109375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="54" customWidth="1"/>
+    <col min="3" max="9" width="10.7109375" style="35" customWidth="1"/>
+    <col min="10" max="16384" width="10.7109375" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -5200,668 +5206,668 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="33">
         <v>42355</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="35" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="37" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="33">
         <v>42355</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="35" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="33">
         <v>42355</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="35" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="50" t="s">
         <v>366</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="33">
         <v>42355</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="37" t="s">
+      <c r="A6" s="42"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="33">
         <v>42355</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="39" t="s">
+      <c r="A7" s="42"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="33">
         <v>42355</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="37" t="s">
+      <c r="A8" s="42"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="33">
         <v>42355</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="37" t="s">
+      <c r="A9" s="43"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="33">
         <v>42355</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="35" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="33">
         <v>42355</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="35" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="33">
         <v>42355</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="40" t="s">
+      <c r="I11" s="35" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="33">
         <v>42355</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="35" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="37" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="33">
         <v>42355</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="35" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="37" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="33">
         <v>42355</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="40" t="s">
+      <c r="I14" s="35" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="39" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="33">
         <v>42355</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="40" t="s">
+      <c r="I15" s="35" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="33">
         <v>42355</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I16" s="40" t="s">
+      <c r="I16" s="35" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="33">
         <v>42355</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="35" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="39" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="33">
         <v>42355</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="35" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="33">
         <v>42355</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="35" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="33">
         <v>42355</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="55" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="33">
         <v>42355</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="35" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="33">
         <v>42355</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G22" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="40" t="s">
+      <c r="I22" s="35" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="33">
         <v>42355</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I23" s="40" t="s">
+      <c r="I23" s="35" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="33">
         <v>42355</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I24" s="40" t="s">
+      <c r="I24" s="35" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="39" t="s">
+      <c r="A25" s="40"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="33">
         <v>42355</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="35" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="53" t="s">
         <v>181</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E26" s="33">
         <v>42356</v>
       </c>
-      <c r="F26" s="39" t="s">
+      <c r="F26" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="39" t="s">
+      <c r="G26" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="53" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="E27" s="38">
+      <c r="E27" s="33">
         <v>42356</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="G27" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E28" s="33">
         <v>42357</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="39" t="s">
+      <c r="G28" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I28" s="40" t="s">
+      <c r="I28" s="35" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="33">
         <v>42358</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="35" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5961,15 +5967,15 @@
       <c r="G2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="45" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="56" t="s">
         <v>373</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -5989,8 +5995,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="17" t="s">
         <v>214</v>
       </c>
@@ -6008,8 +6014,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="17" t="s">
         <v>216</v>
       </c>
@@ -6027,10 +6033,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="57" t="s">
         <v>218</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="44" t="s">
         <v>374</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -6050,7 +6056,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="57"/>
       <c r="C7" s="17" t="s">
         <v>214</v>
       </c>
@@ -6120,10 +6126,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="59" t="s">
         <v>226</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -6146,8 +6152,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="17" t="s">
         <v>216</v>
       </c>
@@ -6189,7 +6195,7 @@
       <c r="G12" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="49" t="s">
+      <c r="I12" s="44" t="s">
         <v>371</v>
       </c>
     </row>
@@ -6215,7 +6221,7 @@
       <c r="G13" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="49" t="s">
+      <c r="I13" s="44" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6241,7 +6247,7 @@
       <c r="G14" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="49" t="s">
+      <c r="I14" s="44" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6353,7 +6359,7 @@
         <v>92</v>
       </c>
       <c r="H3" s="17"/>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="35" t="s">
         <v>371</v>
       </c>
     </row>
@@ -6366,8 +6372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6412,10 +6418,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="59" t="s">
         <v>213</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -6438,8 +6444,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="17" t="s">
         <v>246</v>
       </c>
@@ -6460,8 +6466,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="17" t="s">
         <v>248</v>
       </c>
@@ -6503,7 +6509,7 @@
       <c r="G5" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="49" t="s">
+      <c r="I5" s="44" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6555,7 +6561,7 @@
       <c r="G7" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="49" t="s">
+      <c r="I7" s="44" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6581,6 +6587,9 @@
       <c r="G8" s="17" t="s">
         <v>92</v>
       </c>
+      <c r="I8" s="17" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
@@ -6604,7 +6613,7 @@
       <c r="G9" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="49" t="s">
+      <c r="I9" s="44" t="s">
         <v>372</v>
       </c>
     </row>

</xml_diff>